<commit_message>
improved tests for excel import/export/template
git-svn-id: https://svn.fao.org/projects/ruralinvest/RIV4/trunk@67064 d7fa552c-c32d-11e1-9f2d-6d39f2a56844
</commit_message>
<xml_diff>
--- a/RIV4-tests/src/test/resources/imports/project/block-nig.xlsx
+++ b/RIV4-tests/src/test/resources/imports/project/block-nig.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>User charge</t>
   </si>
@@ -110,6 +110,14 @@
   </si>
   <si>
     <t>Exactly None</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -160,11 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,7 +507,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -620,8 +629,8 @@
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -652,8 +661,8 @@
       <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="B9">
-        <v>0</v>
+      <c r="B9" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -774,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="3">
         <f>C14*F14</f>

</xml_diff>